<commit_message>
tercer commit de prueba
</commit_message>
<xml_diff>
--- a/Fechas_hoy_iLOG.xlsx
+++ b/Fechas_hoy_iLOG.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>18/05/2021 07:24:03</t>
+          <t>18/05/2021 12:27:02</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>40%</t>
+          <t>38%</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>18/05/2021 08:59:31</t>
+          <t>19/05/2021 08:54:49</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>18/05/2021 09:04:54</t>
+          <t>19/05/2021 09:07:21</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -533,7 +533,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>18/05/2021 08:45:20</t>
+          <t>19/05/2021 08:46:14</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -551,16 +551,8 @@
           <t>865284040300166</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>17/05/2021 21:14:03</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>05%</t>
-        </is>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -573,12 +565,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>18/05/2021 08:48:37</t>
+          <t>19/05/2021 09:01:22</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>100%</t>
+          <t>98%</t>
         </is>
       </c>
     </row>
@@ -593,12 +585,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>18/05/2021 09:17:42</t>
+          <t>19/05/2021 09:14:27</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>52%</t>
+          <t>42%</t>
         </is>
       </c>
     </row>
@@ -613,7 +605,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>18/05/2021 08:57:20</t>
+          <t>19/05/2021 08:57:16</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -645,7 +637,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>18/05/2021 09:01:43</t>
+          <t>19/05/2021 09:12:19</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -677,7 +669,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>18/05/2021 07:53:58</t>
+          <t>19/05/2021 08:49:14</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -697,7 +689,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>18/05/2021 09:04:46</t>
+          <t>19/05/2021 08:49:43</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -717,7 +709,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>18/05/2021 09:20:26</t>
+          <t>19/05/2021 09:16:58</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -737,12 +729,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>18/05/2021 07:36:48</t>
+          <t>19/05/2021 09:14:33</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>95%</t>
+          <t>100%</t>
         </is>
       </c>
     </row>
@@ -755,16 +747,8 @@
           <t>865284040234225</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>18/05/2021 03:52:00</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -789,12 +773,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>18/05/2021 09:01:36</t>
+          <t>19/05/2021 09:09:53</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>89%</t>
+          <t>90%</t>
         </is>
       </c>
     </row>
@@ -809,7 +793,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>18/05/2021 08:35:12</t>
+          <t>19/05/2021 08:19:55</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -829,7 +813,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>17/05/2021 19:12:14</t>
+          <t>18/05/2021 19:12:53</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -849,12 +833,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>18/05/2021 08:43:20</t>
+          <t>19/05/2021 08:33:46</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>72%</t>
         </is>
       </c>
     </row>
@@ -869,12 +853,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>18/05/2021 09:00:35</t>
+          <t>19/05/2021 09:04:20</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>88%</t>
+          <t>86%</t>
         </is>
       </c>
     </row>
@@ -889,12 +873,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>18/05/2021 01:09:08</t>
+          <t>19/05/2021 01:09:17</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>27%</t>
+          <t>28%</t>
         </is>
       </c>
     </row>
@@ -921,12 +905,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>18/05/2021 09:03:03</t>
+          <t>19/05/2021 08:21:50</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>37%</t>
+          <t>36%</t>
         </is>
       </c>
     </row>

</xml_diff>